<commit_message>
Add .gitignore: ignore macOS metadata, Excel temp files, raw JSON
</commit_message>
<xml_diff>
--- a/ctgov_mapping_v1.xlsx
+++ b/ctgov_mapping_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanfung/Library/Mobile Documents/com~apple~CloudDocs/UCL MSc DSML/MSc Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB1CDA5-5BDB-6947-BA46-3F189A0022CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9AC0AE-BCF1-374C-ADDE-6FD68952B198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14800" yWindow="760" windowWidth="19620" windowHeight="21580" xr2:uid="{A6ED2628-BB2B-C742-ACBD-73174A164BBD}"/>
+    <workbookView xWindow="560" yWindow="760" windowWidth="19620" windowHeight="21580" xr2:uid="{A6ED2628-BB2B-C742-ACBD-73174A164BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="113">
   <si>
     <t>variable_wishlist</t>
   </si>
@@ -515,9 +515,6 @@
     </r>
   </si>
   <si>
-    <t>If list contains "CHILD" → peds;  if list contains "ADULT? → adult</t>
-  </si>
-  <si>
     <t>PHASE1, PHASE2, PHASE3, PHASE4</t>
   </si>
   <si>
@@ -652,6 +649,9 @@
   </si>
   <si>
     <t>resultsSection.adverseEventsModule.seriousEvents | resultsSection.adverseEventsModule.otherEvents</t>
+  </si>
+  <si>
+    <t>If list contains "CHILD" → peds;  if list contains "ADULT" → adult</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED433BD-12EC-B84D-8A71-386670E0261B}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1130,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1204,7 +1204,7 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1292,7 +1292,7 @@
         <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1308,7 +1308,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1332,13 +1332,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1352,7 +1352,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1426,7 +1426,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>66</v>
@@ -1440,13 +1440,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1512,7 +1512,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1522,13 +1522,13 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1629,7 +1629,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>66</v>
@@ -1694,7 +1694,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
@@ -1704,7 +1704,9 @@
       <c r="C45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
@@ -1719,7 +1721,7 @@
         <v>68</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1905,55 +1907,55 @@
         <v>50</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" t="s">
         <v>100</v>
-      </c>
-      <c r="B61" t="s">
-        <v>101</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" t="s">
         <v>106</v>
-      </c>
-      <c r="B63" t="s">
-        <v>107</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>

</xml_diff>

<commit_message>
Update ctgov_mapping_v1.xlsx with latest mappings
</commit_message>
<xml_diff>
--- a/ctgov_mapping_v1.xlsx
+++ b/ctgov_mapping_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanfung/Library/Mobile Documents/com~apple~CloudDocs/UCL MSc DSML/MSc Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B601C0-DF5A-5D4E-8ACD-72B8927274F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF45027-C9D1-984D-B824-56EB52FC41BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="760" windowWidth="19620" windowHeight="21580" xr2:uid="{A6ED2628-BB2B-C742-ACBD-73174A164BBD}"/>
+    <workbookView xWindow="15760" yWindow="760" windowWidth="18080" windowHeight="21580" xr2:uid="{A6ED2628-BB2B-C742-ACBD-73174A164BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
   <si>
     <t>variable_wishlist</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>NONE / SINGLE / DOUBLE / TRIPLE / QUADRUPLE</t>
-  </si>
-  <si>
-    <t>ISO date (YYYY-MM or YYYY-MM-DD)</t>
   </si>
   <si>
     <t>study type</t>
@@ -527,9 +524,36 @@
     <t>protocolSection.eligibilityModule.eligibilityCriteria</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Parse both ISO strings, then </t>
-    </r>
+    <t>len(locations)</t>
+  </si>
+  <si>
+    <t>Allocation (Randomised / Non-randomised)</t>
+  </si>
+  <si>
+    <t>protocolSection.designModule.designInfo.allocation</t>
+  </si>
+  <si>
+    <t>protocolSection.oversightModule.isFdaRegulatedDrug</t>
+  </si>
+  <si>
+    <t>N/A means no upper limit</t>
+  </si>
+  <si>
+    <t>RANDOMIZED, NON_RANDOMIZED, N_A</t>
+  </si>
+  <si>
+    <t>FDA-regulated drug</t>
+  </si>
+  <si>
+    <t>FDA-regulated device</t>
+  </si>
+  <si>
+    <t>protocolSection.oversightModule.isFdaRegulatedDevice</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -537,7 +561,7 @@
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
       </rPr>
-      <t>duration = primaryCompletion − start</t>
+      <t>"DRUG"</t>
     </r>
     <r>
       <rPr>
@@ -547,46 +571,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> in days. Both fields are present in every record</t>
-    </r>
-  </si>
-  <si>
-    <t>protocolSection.statusModule.startDateStruct.date | protocolSection.statusModule.primaryCompletionDateStruct.date</t>
-  </si>
-  <si>
-    <t>resultsSection.participantFlowModule.participantFlowMilestones</t>
-  </si>
-  <si>
-    <t>len(locations)</t>
-  </si>
-  <si>
-    <t>Allocation (Randomised / Non-randomised)</t>
-  </si>
-  <si>
-    <t>protocolSection.designModule.designInfo.allocation</t>
-  </si>
-  <si>
-    <t>protocolSection.oversightModule.isFdaRegulatedDrug</t>
-  </si>
-  <si>
-    <t>N/A means no upper limit</t>
-  </si>
-  <si>
-    <t>RANDOMIZED, NON_RANDOMIZED, N_A</t>
-  </si>
-  <si>
-    <t>FDA-regulated drug</t>
-  </si>
-  <si>
-    <t>FDA-regulated device</t>
-  </si>
-  <si>
-    <t>protocolSection.oversightModule.isFdaRegulatedDevice</t>
-  </si>
-  <si>
-    <t>Yes/No</t>
-  </si>
-  <si>
+      <t xml:space="preserve">, </t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -594,7 +580,7 @@
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
       </rPr>
-      <t>"DRUG"</t>
+      <t>"BIOLOGICAL"</t>
     </r>
     <r>
       <rPr>
@@ -613,42 +599,29 @@
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
       </rPr>
-      <t>"BIOLOGICAL"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
       <t>"DEVICE"</t>
     </r>
   </si>
   <si>
-    <t>Requires results-posted-trials: Compute (screened-started)/ screened using "assessed for eligibility" vs "started"</t>
-  </si>
-  <si>
-    <t>Requires results-posted-trials: Compute (started-completed)/ started from milestone counts</t>
-  </si>
-  <si>
-    <t>resultsSection.adverseEventsModule.seriousEvents | resultsSection.adverseEventsModule.otherEvents</t>
-  </si>
-  <si>
     <t>If list contains "CHILD" → peds;  if list contains "ADULT" → adult</t>
   </si>
   <si>
     <t>protocolSection.oversightModule.oversightHasDmc</t>
+  </si>
+  <si>
+    <t>ISO date (YYYY-MM or YYYY-MM-DD); parse later</t>
+  </si>
+  <si>
+    <t>completion date</t>
+  </si>
+  <si>
+    <t>protocolSection.statusModule.primaryCompletionDateStruct.date</t>
+  </si>
+  <si>
+    <t>Use this and above feature to compute Treament duration</t>
+  </si>
+  <si>
+    <t>see new addition;  this is computed using study start date and completion date</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED433BD-12EC-B84D-8A71-386670E0261B}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1123,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1158,13 +1131,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -1172,13 +1145,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1186,7 +1159,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -1194,13 +1167,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1208,7 +1181,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1216,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1232,13 +1205,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
@@ -1252,7 +1225,7 @@
         <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1260,7 +1233,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
@@ -1271,13 +1244,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
         <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1285,10 +1258,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -1296,13 +1269,13 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1310,7 +1283,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,23 +1291,23 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1342,24 +1315,21 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1367,13 +1337,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
         <v>80</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1381,13 +1351,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1405,22 +1375,13 @@
       <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
       <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1428,7 +1389,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1436,7 +1397,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1444,7 +1405,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1460,7 +1421,7 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1468,7 +1429,7 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,18 +1437,15 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
-        <v>109</v>
-      </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1495,7 +1453,7 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1503,7 +1461,7 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,7 +1469,7 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1527,13 +1485,13 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.25">
@@ -1541,13 +1499,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,7 +1513,7 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1563,7 +1521,7 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1571,7 +1529,7 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1579,7 +1537,7 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1587,7 +1545,7 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1595,12 +1553,12 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>48</v>
@@ -1617,120 +1575,134 @@
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
         <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
         <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
         <v>50</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C58" t="s">
         <v>50</v>
       </c>
+      <c r="D58" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
         <v>50</v>
       </c>
-      <c r="D59" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
         <v>50</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
         <v>50</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
         <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C1048576 D55">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="missing">
       <formula>NOT(ISERROR(SEARCH("missing",C1)))</formula>
     </cfRule>

</xml_diff>